<commit_message>
LVBR-213 Codelijst zakelijk recht
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/zakelijkrecht/zakelijkrecht.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/zakelijkrecht/zakelijkrecht.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,16 +428,13 @@
         <v>topConceptOf</v>
       </c>
       <c r="I1" t="str">
-        <v>altLabel</v>
+        <v>belongsTo</v>
       </c>
       <c r="J1" t="str">
+        <v>hasTopConcept</v>
+      </c>
+      <c r="K1" t="str">
         <v>theme</v>
-      </c>
-      <c r="K1" t="str">
-        <v>belongsTo</v>
-      </c>
-      <c r="L1" t="str">
-        <v>hasTopConcept</v>
       </c>
     </row>
     <row r="2">
@@ -474,9 +471,6 @@
       <c r="K2" t="str">
         <v>null</v>
       </c>
-      <c r="L2" t="str">
-        <v>null</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -512,9 +506,6 @@
       <c r="K3" t="str">
         <v>null</v>
       </c>
-      <c r="L3" t="str">
-        <v>null</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -542,15 +533,12 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zakelijkrecht</v>
       </c>
       <c r="I4" t="str">
-        <v>Gebrek dat leidt tot vochtindringing</v>
+        <v>null</v>
       </c>
       <c r="J4" t="str">
-        <v>http://www.eionet.europa.eu/gemet/theme/5</v>
+        <v>null</v>
       </c>
       <c r="K4" t="str">
-        <v>null</v>
-      </c>
-      <c r="L4" t="str">
         <v>null</v>
       </c>
     </row>
@@ -588,9 +576,6 @@
       <c r="K5" t="str">
         <v>null</v>
       </c>
-      <c r="L5" t="str">
-        <v>null</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -618,21 +603,18 @@
         <v>null</v>
       </c>
       <c r="I6" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-zakelijkrecht</v>
       </c>
       <c r="J6" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/erfpacht|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/opstal|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/volle_eigendom|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/vruchtgebruik</v>
+      </c>
+      <c r="K6" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
-      </c>
-      <c r="K6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-zakelijkrecht</v>
-      </c>
-      <c r="L6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/erfpacht|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/opstal|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/volle_eigendom|https://data.omgeving.vlaanderen.be/id/concept/zakelijkrecht/vruchtgebruik</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>